<commit_message>
adding text and updating  inline code to match
</commit_message>
<xml_diff>
--- a/inputs/TheDataCenter_PopulationbyParish.xlsx
+++ b/inputs/TheDataCenter_PopulationbyParish.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://datacenterresearch-my.sharepoint.com/personal/haleight_datacenterresearch_org/Documents/Desktop/Working Directory/Who-Lives/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://datacenterresearch-my.sharepoint.com/personal/anissah_datacenterresearch_org/Documents/DC_Projects/Who-Lives/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F85C25A-55FA-4FB9-ADDB-ECA3049F70DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{56898902-0AB5-49D4-A7FF-86B6265902E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{871D7D4E-71F9-46AE-81EC-A7AC154C0055}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1440" windowWidth="16875" windowHeight="10163" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37620" yWindow="2460" windowWidth="23016" windowHeight="11952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Jefferson</t>
   </si>
@@ -53,65 +56,26 @@
     <t>St. James</t>
   </si>
   <si>
-    <t>St. Tammany</t>
+    <t>St. John the Baptist</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>metro_pop</t>
   </si>
   <si>
     <t>Metro Area total</t>
   </si>
-  <si>
-    <t>Census 1980</t>
-  </si>
-  <si>
-    <t>Census 1990</t>
-  </si>
-  <si>
-    <t>Census 2000</t>
-  </si>
-  <si>
-    <t>Census 2010</t>
-  </si>
-  <si>
-    <t>Census 2020</t>
-  </si>
-  <si>
-    <t>Estimate 2021</t>
-  </si>
-  <si>
-    <t>Estimate 2022</t>
-  </si>
-  <si>
-    <t>Estimate 2023</t>
-  </si>
-  <si>
-    <t>St. John the Baptist</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -124,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -132,37 +96,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,6 +117,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,305 +409,307 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F514D9-282F-4A7C-A782-4A86A9163C82}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8AB0B98-8AE7-41B8-A0C6-69695EF27476}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.76171875" customWidth="1"/>
+    <col min="5" max="5" width="10.05859375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.234375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1980</v>
+      </c>
+      <c r="B2">
         <v>454592</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2">
         <v>557515</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2">
         <v>26049</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2">
         <v>64097</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2">
         <v>37259</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2">
         <v>21495</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2">
         <v>31924</v>
       </c>
-      <c r="I2" s="5">
-        <v>110869</v>
-      </c>
-      <c r="J2" s="6">
-        <v>1303800</v>
+      <c r="I2">
+        <v>1192931</v>
+      </c>
+      <c r="J2">
+        <v>1192931</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
         <v>448306</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
         <v>496938</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3">
         <v>25575</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3">
         <v>66631</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3">
         <v>42437</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3">
         <v>20879</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3">
         <v>39996</v>
       </c>
-      <c r="I3" s="5">
-        <v>144508</v>
-      </c>
-      <c r="J3" s="6">
-        <v>1285270</v>
+      <c r="I3">
+        <v>1140762</v>
+      </c>
+      <c r="J3">
+        <v>1140762</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+      <c r="B4">
         <v>455466</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4">
         <v>484674</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4">
         <v>26757</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4">
         <v>67229</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4">
         <v>48072</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4">
         <v>21216</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4">
         <v>43044</v>
       </c>
-      <c r="I4" s="5">
-        <v>191268</v>
-      </c>
-      <c r="J4" s="6">
-        <f>SUM(B4:I4)</f>
-        <v>1337726</v>
+      <c r="I4">
+        <v>1146458</v>
+      </c>
+      <c r="J4">
+        <v>1146458</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2010</v>
+      </c>
+      <c r="B5">
         <v>432552</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5">
         <v>343829</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <v>23042</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
         <v>35897</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5">
         <v>52780</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5">
         <v>22102</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5">
         <v>45924</v>
       </c>
-      <c r="I5" s="5">
-        <v>233740</v>
-      </c>
-      <c r="J5" s="6">
-        <f>SUM(B5:I5)</f>
-        <v>1189866</v>
+      <c r="I5">
+        <v>956126</v>
+      </c>
+      <c r="J5">
+        <v>956126</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6">
         <v>440781</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6">
         <v>383997</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6">
         <v>23515</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6">
         <v>43764</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6">
         <v>52549</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6">
         <v>20192</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6">
         <v>42477</v>
       </c>
-      <c r="I6" s="5">
-        <v>264570</v>
-      </c>
-      <c r="J6" s="6">
-        <f>SUM(B6:I6)</f>
-        <v>1271845</v>
+      <c r="I6">
+        <v>1007275</v>
+      </c>
+      <c r="J6">
+        <v>1007275</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2021</v>
+      </c>
+      <c r="B7">
         <v>434134</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7">
         <v>377346</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7">
         <v>23310</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7">
         <v>44324</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7">
         <v>52470</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7">
         <v>19794</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7">
         <v>42109</v>
       </c>
-      <c r="I7" s="5">
-        <v>270147</v>
-      </c>
-      <c r="J7" s="6">
-        <f>SUM(B7:I7)</f>
-        <v>1263634</v>
+      <c r="I7">
+        <v>993487</v>
+      </c>
+      <c r="J7">
+        <v>993487</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="5">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2022</v>
+      </c>
+      <c r="B8">
         <v>426030</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8">
         <v>369917</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8">
         <v>22618</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8">
         <v>44419</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8">
         <v>51058</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8">
         <v>19388</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8">
         <v>39955</v>
       </c>
-      <c r="I8" s="5">
-        <v>273237</v>
-      </c>
-      <c r="J8" s="6">
-        <f t="shared" ref="J8:J9" si="0">SUM(B8:I8)</f>
-        <v>1246622</v>
+      <c r="I8">
+        <v>973385</v>
+      </c>
+      <c r="J8">
+        <v>973385</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2023</v>
+      </c>
+      <c r="B9">
         <v>421777</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9">
         <v>364136</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9">
         <v>22386</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9">
         <v>44463</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9">
         <v>50620</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9">
         <v>19191</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9">
         <v>39592</v>
       </c>
-      <c r="I9" s="5">
-        <v>275583</v>
-      </c>
-      <c r="J9" s="6">
-        <f t="shared" si="0"/>
-        <v>1237748</v>
+      <c r="I9">
+        <v>962165</v>
+      </c>
+      <c r="J9">
+        <v>962165</v>
       </c>
     </row>
   </sheetData>
@@ -773,6 +718,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07a26812-85d3-4425-992a-629e808a49a8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="26ce723e-735e-4eb2-8b68-455e42ea4533" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D504898F6C39A345BE7DC6B777612B12" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c903bc8010700ac468ab3bd9da055d38">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07a26812-85d3-4425-992a-629e808a49a8" xmlns:ns3="26ce723e-735e-4eb2-8b68-455e42ea4533" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0360ef8260ba8797d0d24b6430bbf7d" ns2:_="" ns3:_="">
     <xsd:import namespace="07a26812-85d3-4425-992a-629e808a49a8"/>
@@ -1027,27 +992,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07a26812-85d3-4425-992a-629e808a49a8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="26ce723e-735e-4eb2-8b68-455e42ea4533" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7EAAFCA-5D2D-4BBA-8475-74562EB4073E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{122DFA70-9467-44B1-A8AC-281E77905B99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="07a26812-85d3-4425-992a-629e808a49a8"/>
+    <ds:schemaRef ds:uri="26ce723e-735e-4eb2-8b68-455e42ea4533"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E558CA1F-5D86-4254-8979-C085C732D5A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1064,23 +1028,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{122DFA70-9467-44B1-A8AC-281E77905B99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="07a26812-85d3-4425-992a-629e808a49a8"/>
-    <ds:schemaRef ds:uri="26ce723e-735e-4eb2-8b68-455e42ea4533"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7EAAFCA-5D2D-4BBA-8475-74562EB4073E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>